<commit_message>
reverted to using old investor codes
</commit_message>
<xml_diff>
--- a/modified_GP_CRM.xlsx
+++ b/modified_GP_CRM.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gpfundsolutions-my.sharepoint.com/personal/ppark_gpes_com/Documents/Desktop/doc_generator/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6939A1E4FDDBC82CE72D4CAFA5292B817979CCF6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DA57622-8954-483B-8672-355CAFF04AFA}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Investor" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -73,424 +67,424 @@
     <t>Subscription</t>
   </si>
   <si>
-    <t>JoSmDePaVLP</t>
-  </si>
-  <si>
-    <t>JoSmDePaIVLP</t>
-  </si>
-  <si>
-    <t>JoSmStEqPaLP</t>
-  </si>
-  <si>
-    <t>JoSmReEsIILP</t>
-  </si>
-  <si>
-    <t>JoSmDePaVILP2</t>
-  </si>
-  <si>
-    <t>JoSmCaPaI</t>
-  </si>
-  <si>
-    <t>JoSmDePaVILP1</t>
-  </si>
-  <si>
-    <t>JoSmDePaIILP2</t>
-  </si>
-  <si>
-    <t>JoSmStEqFuIILP</t>
-  </si>
-  <si>
-    <t>JoSmGrFuVILP3</t>
-  </si>
-  <si>
-    <t>JoSmGrFuVILP2</t>
-  </si>
-  <si>
-    <t>JoSmReEsIVLP</t>
-  </si>
-  <si>
-    <t>JoSmGrFuVLP</t>
-  </si>
-  <si>
-    <t>JoSmCaPaII</t>
-  </si>
-  <si>
-    <t>JoSmMaFuI</t>
-  </si>
-  <si>
-    <t>JoSmDePaIILP1</t>
-  </si>
-  <si>
-    <t>JoSmFuPrLP</t>
-  </si>
-  <si>
-    <t>JoSmStPaIILP</t>
-  </si>
-  <si>
-    <t>JoSmGrFuVILP1</t>
-  </si>
-  <si>
-    <t>EmJoGrFuVILP3</t>
-  </si>
-  <si>
-    <t>EmJoGrFuVILP2</t>
-  </si>
-  <si>
-    <t>EmJoReEsIILP</t>
-  </si>
-  <si>
-    <t>EmJoDePaVILP2</t>
-  </si>
-  <si>
-    <t>EmJoReEsIVLP</t>
-  </si>
-  <si>
-    <t>EmJoCaPaI</t>
-  </si>
-  <si>
-    <t>EmJoDePaVLP</t>
-  </si>
-  <si>
-    <t>EmJoGrFuVLP</t>
-  </si>
-  <si>
-    <t>EmJoCaPaII</t>
-  </si>
-  <si>
-    <t>EmJoDePaVILP1</t>
-  </si>
-  <si>
-    <t>EmJoDePaIVLP</t>
-  </si>
-  <si>
-    <t>EmJoDePaIILP2</t>
-  </si>
-  <si>
-    <t>EmJoStEqFuIILP</t>
-  </si>
-  <si>
-    <t>EmJoMaFuI</t>
-  </si>
-  <si>
-    <t>EmJoStPaIILP</t>
-  </si>
-  <si>
-    <t>EmJoGrFuVILP1</t>
-  </si>
-  <si>
-    <t>EmJoStEqPaLP</t>
-  </si>
-  <si>
-    <t>EmJoDePaIILP1</t>
-  </si>
-  <si>
-    <t>MiWiGrFuVILP3</t>
-  </si>
-  <si>
-    <t>MiWiGrFuVILP2</t>
-  </si>
-  <si>
-    <t>MiWiReEsIILP</t>
-  </si>
-  <si>
-    <t>MiWiDePaVILP2</t>
-  </si>
-  <si>
-    <t>MiWiReEsIVLP</t>
-  </si>
-  <si>
-    <t>MiWiGrFuVLP</t>
-  </si>
-  <si>
-    <t>MiWiCaPaII</t>
-  </si>
-  <si>
-    <t>MiWiDePaVILP1</t>
-  </si>
-  <si>
-    <t>MiWiDePaIVLP</t>
-  </si>
-  <si>
-    <t>MiWiDePaIILP2</t>
-  </si>
-  <si>
-    <t>MiWiStEqFuIILP</t>
-  </si>
-  <si>
-    <t>MiWiMaFuI</t>
-  </si>
-  <si>
-    <t>MiWiStPaIILP</t>
-  </si>
-  <si>
-    <t>MiWiGrFuVILP1</t>
-  </si>
-  <si>
-    <t>MiWiStEqPaLP</t>
-  </si>
-  <si>
-    <t>MiWiDePaIILP1</t>
-  </si>
-  <si>
-    <t>SoBrGrFuVILP3</t>
-  </si>
-  <si>
-    <t>SoBrGrFuVILP2</t>
-  </si>
-  <si>
-    <t>SoBrReEsIILP</t>
-  </si>
-  <si>
-    <t>SoBrDePaVILP2</t>
-  </si>
-  <si>
-    <t>SoBrReEsIVLP</t>
-  </si>
-  <si>
-    <t>SoBrDePaVLP</t>
-  </si>
-  <si>
-    <t>SoBrGrFuVLP</t>
-  </si>
-  <si>
-    <t>SoBrCaPaII</t>
-  </si>
-  <si>
-    <t>SoBrDePaVILP1</t>
-  </si>
-  <si>
-    <t>SoBrDePaIVLP</t>
-  </si>
-  <si>
-    <t>SoBrDePaIILP2</t>
-  </si>
-  <si>
-    <t>SoBrStEqFuIILP</t>
-  </si>
-  <si>
-    <t>SoBrMaFuI</t>
-  </si>
-  <si>
-    <t>SoBrStPaIILP</t>
-  </si>
-  <si>
-    <t>SoBrGrFuVILP1</t>
-  </si>
-  <si>
-    <t>SoBrStEqPaLP</t>
-  </si>
-  <si>
-    <t>SoBrDePaIILP1</t>
-  </si>
-  <si>
-    <t>DaDaGrFuVILP3</t>
-  </si>
-  <si>
-    <t>DaDaGrFuVILP2</t>
-  </si>
-  <si>
-    <t>DaDaDePaVILP2</t>
-  </si>
-  <si>
-    <t>DaDaReEsIVLP</t>
-  </si>
-  <si>
-    <t>DaDaCaPaI</t>
-  </si>
-  <si>
-    <t>DaDaGrFuVLP</t>
-  </si>
-  <si>
-    <t>DaDaCaPaII</t>
-  </si>
-  <si>
-    <t>DaDaDePaVILP1</t>
-  </si>
-  <si>
-    <t>DaDaDePaIVLP</t>
-  </si>
-  <si>
-    <t>DaDaDePaIILP2</t>
-  </si>
-  <si>
-    <t>DaDaMaFuI</t>
-  </si>
-  <si>
-    <t>DaDaStPaIILP</t>
-  </si>
-  <si>
-    <t>DaDaGrFuVILP1</t>
-  </si>
-  <si>
-    <t>DaDaStEqPaLP</t>
-  </si>
-  <si>
-    <t>DaDaDePaIILP1</t>
-  </si>
-  <si>
-    <t>OlMiGrFuVILP3</t>
-  </si>
-  <si>
-    <t>OlMiGrFuVILP2</t>
-  </si>
-  <si>
-    <t>OlMiDePaVILP2</t>
-  </si>
-  <si>
-    <t>OlMiDePaVLP</t>
-  </si>
-  <si>
-    <t>OlMiCaPaI</t>
-  </si>
-  <si>
-    <t>OlMiGrFuVLP</t>
-  </si>
-  <si>
-    <t>OlMiCaPaII</t>
-  </si>
-  <si>
-    <t>OlMiDePaVILP1</t>
-  </si>
-  <si>
-    <t>OlMiDePaIVLP</t>
-  </si>
-  <si>
-    <t>OlMiMaFuI</t>
-  </si>
-  <si>
-    <t>OlMiStPaIILP</t>
-  </si>
-  <si>
-    <t>OlMiGrFuVILP1</t>
-  </si>
-  <si>
-    <t>OlMiStEqPaLP</t>
-  </si>
-  <si>
-    <t>JaWiGrFuVILP2</t>
-  </si>
-  <si>
-    <t>JaWiReEsIILP</t>
-  </si>
-  <si>
-    <t>JaWiDePaVILP2</t>
-  </si>
-  <si>
-    <t>JaWiReEsIVLP</t>
-  </si>
-  <si>
-    <t>JaWiDePaVLP</t>
-  </si>
-  <si>
-    <t>JaWiGrFuVLP</t>
-  </si>
-  <si>
-    <t>JaWiCaPaII</t>
-  </si>
-  <si>
-    <t>JaWiDePaVILP1</t>
-  </si>
-  <si>
-    <t>JaWiDePaIVLP</t>
-  </si>
-  <si>
-    <t>JaWiDePaIILP2</t>
-  </si>
-  <si>
-    <t>JaWiGrFuVILP1</t>
-  </si>
-  <si>
-    <t>JaWiDePaIILP1</t>
-  </si>
-  <si>
-    <t>IsMoGrFuVILP3</t>
-  </si>
-  <si>
-    <t>IsMoGrFuVILP2</t>
-  </si>
-  <si>
-    <t>IsMoDePaVILP2</t>
-  </si>
-  <si>
-    <t>IsMoReEsIVLP</t>
-  </si>
-  <si>
-    <t>IsMoGrFuVLP</t>
-  </si>
-  <si>
-    <t>IsMoCaPaII</t>
-  </si>
-  <si>
-    <t>IsMoDePaIVLP</t>
-  </si>
-  <si>
-    <t>IsMoStEqFuIILP</t>
-  </si>
-  <si>
-    <t>IsMoMaFuI</t>
-  </si>
-  <si>
-    <t>IsMoStPaIILP</t>
-  </si>
-  <si>
-    <t>IsMoGrFuVILP1</t>
-  </si>
-  <si>
-    <t>IsMoStEqPaLP</t>
-  </si>
-  <si>
-    <t>BeTaGrFuVILP3</t>
-  </si>
-  <si>
-    <t>BeTaGrFuVILP2</t>
-  </si>
-  <si>
-    <t>BeTaReEsIILP</t>
-  </si>
-  <si>
-    <t>BeTaDePaVILP2</t>
-  </si>
-  <si>
-    <t>BeTaReEsIVLP</t>
-  </si>
-  <si>
-    <t>BeTaGrFuVLP</t>
-  </si>
-  <si>
-    <t>BeTaCaPaII</t>
-  </si>
-  <si>
-    <t>BeTaDePaVILP1</t>
-  </si>
-  <si>
-    <t>BeTaDePaIVLP</t>
-  </si>
-  <si>
-    <t>BeTaMaFuI</t>
-  </si>
-  <si>
-    <t>BeTaStPaIILP</t>
-  </si>
-  <si>
-    <t>BeTaGrFuVILP1</t>
-  </si>
-  <si>
-    <t>BeTaStEqPaLP</t>
-  </si>
-  <si>
-    <t>BeTaDePaIILP1</t>
-  </si>
-  <si>
-    <t>AvAnGrFuVILP3</t>
-  </si>
-  <si>
-    <t>AvAnMaFuI</t>
-  </si>
-  <si>
-    <t>AvAnStEqPaLP</t>
-  </si>
-  <si>
-    <t>AvAnGrFuVILP2</t>
+    <t>JoSmAEInSBIIPaLP1</t>
+  </si>
+  <si>
+    <t>JoSmAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>JoSmAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>JoSmAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaEuL.</t>
+  </si>
+  <si>
+    <t>JoSmAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>JoSmAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>JoSmAEInPuEqFuLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>JoSmAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaVLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>JoSmAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>JoSmAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>JoSmAEGrFuGPLL</t>
+  </si>
+  <si>
+    <t>JoSmAEImPaLP</t>
+  </si>
+  <si>
+    <t>JoSmAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>EmJoAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>EmJoAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>EmJoAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaEuL.</t>
+  </si>
+  <si>
+    <t>EmJoAEInSBIIPaLP1</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaVLP</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>EmJoAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>EmJoAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>EmJoAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>EmJoAEInPuEqFuLP</t>
+  </si>
+  <si>
+    <t>EmJoAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>EmJoAEImPaLP</t>
+  </si>
+  <si>
+    <t>EmJoAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>EmJoAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>EmJoAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>MiWiAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>MiWiAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>MiWiAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>MiWiAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>MiWiAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>MiWiAEInPaVLP</t>
+  </si>
+  <si>
+    <t>MiWiAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>MiWiAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>MiWiAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>MiWiAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>MiWiAEInPuEqFuLP</t>
+  </si>
+  <si>
+    <t>MiWiAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>MiWiAEImPaLP</t>
+  </si>
+  <si>
+    <t>MiWiAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>MiWiAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>MiWiAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>SoBrAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>SoBrAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>SoBrAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>SoBrAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>SoBrAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>SoBrAEInSBIIPaLP1</t>
+  </si>
+  <si>
+    <t>SoBrAEInPaVLP</t>
+  </si>
+  <si>
+    <t>SoBrAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>SoBrAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>SoBrAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>SoBrAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>SoBrAEInPuEqFuLP</t>
+  </si>
+  <si>
+    <t>SoBrAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>SoBrAEImPaLP</t>
+  </si>
+  <si>
+    <t>SoBrAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>SoBrAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>SoBrAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>DaDaAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>DaDaAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaEuL.</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaVLP</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>DaDaAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>DaDaAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>DaDaAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>DaDaAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>DaDaAEImPaLP</t>
+  </si>
+  <si>
+    <t>DaDaAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>DaDaAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>DaDaAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>OlMiAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>OlMiAEInSBIIPaLP1</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaEuL.</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaVLP</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>OlMiAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>OlMiAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>OlMiAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>OlMiAEImPaLP</t>
+  </si>
+  <si>
+    <t>OlMiAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>OlMiAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>JaWiAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>JaWiAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>JaWiAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>JaWiAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>JaWiAEInSBIIPaLP1</t>
+  </si>
+  <si>
+    <t>JaWiAEInPaVLP</t>
+  </si>
+  <si>
+    <t>JaWiAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>JaWiAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>JaWiAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>JaWiAEMePaIILP2</t>
+  </si>
+  <si>
+    <t>JaWiAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>JaWiAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>IsMoAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>IsMoAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>IsMoAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>IsMoAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>IsMoAEInPaVLP</t>
+  </si>
+  <si>
+    <t>IsMoAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>IsMoAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>IsMoAEInPuEqFuLP</t>
+  </si>
+  <si>
+    <t>IsMoAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>IsMoAEImPaLP</t>
+  </si>
+  <si>
+    <t>IsMoAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>IsMoAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>BeTaAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>BeTaAEInPaVILP2</t>
+  </si>
+  <si>
+    <t>BeTaAEMiMaDeIIGPLP</t>
+  </si>
+  <si>
+    <t>BeTaAEInSBIVPaLP</t>
+  </si>
+  <si>
+    <t>BeTaAEMiMaDeIVGPLP</t>
+  </si>
+  <si>
+    <t>BeTaAEInPaVLP</t>
+  </si>
+  <si>
+    <t>BeTaAEInPaEFIILP</t>
+  </si>
+  <si>
+    <t>BeTaAEInSBIIPaLP2</t>
+  </si>
+  <si>
+    <t>BeTaAEMePaIVLP</t>
+  </si>
+  <si>
+    <t>BeTaAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>BeTaAEImPaLP</t>
+  </si>
+  <si>
+    <t>BeTaAEInPaVILP1</t>
+  </si>
+  <si>
+    <t>BeTaAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>BeTaAEMePaIILP1</t>
+  </si>
+  <si>
+    <t>AvAnAEInPaVILP3</t>
+  </si>
+  <si>
+    <t>AvAnAEPaEXCFLP</t>
+  </si>
+  <si>
+    <t>AvAnAEGrEqPaLP</t>
+  </si>
+  <si>
+    <t>AvAnAEInPaVILP2</t>
   </si>
   <si>
     <t>Debt Partners V LP</t>
@@ -2920,8 +2914,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2984,25 +2978,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3040,7 +3022,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3074,7 +3056,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3109,10 +3090,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3285,17 +3265,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3348,7 +3325,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3398,7 +3375,7 @@
         <v>1217635</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3448,7 +3425,7 @@
         <v>6035657</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3498,7 +3475,7 @@
         <v>5060313</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3548,7 +3525,7 @@
         <v>4765412</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3598,7 +3575,7 @@
         <v>7493499</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3648,7 +3625,7 @@
         <v>9033516</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3698,7 +3675,7 @@
         <v>3225166</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3748,7 +3725,7 @@
         <v>9500136</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -3798,7 +3775,7 @@
         <v>2758032</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3848,7 +3825,7 @@
         <v>4170345</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -3898,7 +3875,7 @@
         <v>4785905</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3948,7 +3925,7 @@
         <v>6294720</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3998,7 +3975,7 @@
         <v>9508504</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -4048,7 +4025,7 @@
         <v>8863167</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -4098,7 +4075,7 @@
         <v>9811990</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -4148,7 +4125,7 @@
         <v>6918590</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4198,7 +4175,7 @@
         <v>5640012</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -4248,7 +4225,7 @@
         <v>5736006</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -4298,7 +4275,7 @@
         <v>9239268</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -4348,7 +4325,7 @@
         <v>9345131</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -4398,7 +4375,7 @@
         <v>3463411</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -4448,7 +4425,7 @@
         <v>5589321</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -4498,7 +4475,7 @@
         <v>5157498</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -4548,7 +4525,7 @@
         <v>3094563</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -4598,7 +4575,7 @@
         <v>4815907</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -4648,7 +4625,7 @@
         <v>7097959</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -4698,7 +4675,7 @@
         <v>609872</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -4748,7 +4725,7 @@
         <v>5500226</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -4798,7 +4775,7 @@
         <v>4450038</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -4848,7 +4825,7 @@
         <v>4876775</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -4898,7 +4875,7 @@
         <v>6118243</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -4948,7 +4925,7 @@
         <v>1277826</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -4998,7 +4975,7 @@
         <v>7060303</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -5048,7 +5025,7 @@
         <v>3521872</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -5098,7 +5075,7 @@
         <v>2662963</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -5148,7 +5125,7 @@
         <v>9085497</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -5198,7 +5175,7 @@
         <v>3490282</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -5248,7 +5225,7 @@
         <v>5703304</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -5298,7 +5275,7 @@
         <v>5826041</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -5348,7 +5325,7 @@
         <v>2659334</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -5398,7 +5375,7 @@
         <v>5378334</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -5448,7 +5425,7 @@
         <v>2476571</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -5498,7 +5475,7 @@
         <v>9266963</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -5548,7 +5525,7 @@
         <v>1830673</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -5598,7 +5575,7 @@
         <v>5506241</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -5648,7 +5625,7 @@
         <v>1093609</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -5698,7 +5675,7 @@
         <v>5447579</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -5748,7 +5725,7 @@
         <v>9531374</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -5798,7 +5775,7 @@
         <v>5520166</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -5848,7 +5825,7 @@
         <v>1215964</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -5898,7 +5875,7 @@
         <v>4532786</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -5948,7 +5925,7 @@
         <v>4498202</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -5998,7 +5975,7 @@
         <v>7081126</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -6048,7 +6025,7 @@
         <v>3981402</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -6098,7 +6075,7 @@
         <v>7861725</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -6148,7 +6125,7 @@
         <v>8722789</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -6198,7 +6175,7 @@
         <v>8195787</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -6248,7 +6225,7 @@
         <v>5390682</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -6298,7 +6275,7 @@
         <v>9698527</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -6348,7 +6325,7 @@
         <v>5229439</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -6398,7 +6375,7 @@
         <v>4195044</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -6448,7 +6425,7 @@
         <v>9610928</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -6498,7 +6475,7 @@
         <v>3342078</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -6548,7 +6525,7 @@
         <v>4901850</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -6598,7 +6575,7 @@
         <v>1983135</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -6648,7 +6625,7 @@
         <v>1256943</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -6698,7 +6675,7 @@
         <v>6462929</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -6748,7 +6725,7 @@
         <v>6482755</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -6798,7 +6775,7 @@
         <v>7829708</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -6848,7 +6825,7 @@
         <v>9924658</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -6898,7 +6875,7 @@
         <v>6795525</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -6948,7 +6925,7 @@
         <v>6677157</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -6998,7 +6975,7 @@
         <v>9664143</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -7048,7 +7025,7 @@
         <v>7109069</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -7098,7 +7075,7 @@
         <v>6303316</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -7148,7 +7125,7 @@
         <v>4387656</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -7198,7 +7175,7 @@
         <v>8648415</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -7248,7 +7225,7 @@
         <v>5562057</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -7298,7 +7275,7 @@
         <v>9277705</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -7348,7 +7325,7 @@
         <v>1337425</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -7398,7 +7375,7 @@
         <v>3117005</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -7448,7 +7425,7 @@
         <v>8654521</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -7498,7 +7475,7 @@
         <v>3113093</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -7548,7 +7525,7 @@
         <v>1651378</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -7598,7 +7575,7 @@
         <v>3700128</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -7648,7 +7625,7 @@
         <v>8141586</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -7698,7 +7675,7 @@
         <v>9074742</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -7748,7 +7725,7 @@
         <v>5440337</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17">
       <c r="A90" t="s">
         <v>105</v>
       </c>
@@ -7798,7 +7775,7 @@
         <v>5632193</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -7848,7 +7825,7 @@
         <v>4259961</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -7898,7 +7875,7 @@
         <v>9092093</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -7948,7 +7925,7 @@
         <v>8145419</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -7998,7 +7975,7 @@
         <v>5174627</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -8048,7 +8025,7 @@
         <v>1136326</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -8098,7 +8075,7 @@
         <v>1154627</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -8148,7 +8125,7 @@
         <v>1399553</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -8198,7 +8175,7 @@
         <v>3004036</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -8248,7 +8225,7 @@
         <v>5703582</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -8298,7 +8275,7 @@
         <v>1839401</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -8348,7 +8325,7 @@
         <v>1156704</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -8398,7 +8375,7 @@
         <v>4681780</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -8448,7 +8425,7 @@
         <v>2912881</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -8498,7 +8475,7 @@
         <v>1621428</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -8548,7 +8525,7 @@
         <v>7657981</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -8598,7 +8575,7 @@
         <v>9901750</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -8648,7 +8625,7 @@
         <v>9270399</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -8698,7 +8675,7 @@
         <v>9465870</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -8748,7 +8725,7 @@
         <v>1809180</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17">
       <c r="A110" t="s">
         <v>125</v>
       </c>
@@ -8798,7 +8775,7 @@
         <v>5946956</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -8848,7 +8825,7 @@
         <v>6652721</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -8898,7 +8875,7 @@
         <v>9989923</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -8948,7 +8925,7 @@
         <v>1643119</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -8998,7 +8975,7 @@
         <v>4346224</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -9048,7 +9025,7 @@
         <v>1060264</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -9098,7 +9075,7 @@
         <v>6004565</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -9148,7 +9125,7 @@
         <v>1722512</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -9198,7 +9175,7 @@
         <v>5344369</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -9248,7 +9225,7 @@
         <v>5043265</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -9298,7 +9275,7 @@
         <v>3835358</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -9348,7 +9325,7 @@
         <v>5454923</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -9398,7 +9375,7 @@
         <v>5931720</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -9448,7 +9425,7 @@
         <v>4664261</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -9498,7 +9475,7 @@
         <v>6417468</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -9548,7 +9525,7 @@
         <v>7926879</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -9598,7 +9575,7 @@
         <v>1867393</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17">
       <c r="A127" t="s">
         <v>142</v>
       </c>
@@ -9648,7 +9625,7 @@
         <v>2787788</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -9698,7 +9675,7 @@
         <v>7599284</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:17">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -9748,7 +9725,7 @@
         <v>1466538</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -9798,7 +9775,7 @@
         <v>4591249</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -9848,7 +9825,7 @@
         <v>4522100</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -9898,7 +9875,7 @@
         <v>2589594</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17">
       <c r="A133" t="s">
         <v>148</v>
       </c>
@@ -9948,7 +9925,7 @@
         <v>8477934</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -9998,7 +9975,7 @@
         <v>8381770</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17">
       <c r="A135" t="s">
         <v>150</v>
       </c>
@@ -10048,7 +10025,7 @@
         <v>1977325</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -10098,7 +10075,7 @@
         <v>3455365</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -10148,7 +10125,7 @@
         <v>946712</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -10198,7 +10175,7 @@
         <v>6413046</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17">
       <c r="A139" t="s">
         <v>154</v>
       </c>
@@ -10248,7 +10225,7 @@
         <v>4922450</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17">
       <c r="A140" t="s">
         <v>155</v>
       </c>
@@ -10298,7 +10275,7 @@
         <v>7841463</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17">
       <c r="A141" t="s">
         <v>156</v>
       </c>

</xml_diff>